<commit_message>
minor modification of check protocol
</commit_message>
<xml_diff>
--- a/Plancheck/check_protocol/defaut.xlsx
+++ b/Plancheck/check_protocol/defaut.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="5400"/>
   </bookViews>
   <sheets>
     <sheet name="General data" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="113">
   <si>
     <t>Name_of check_protocol</t>
   </si>
@@ -1344,8 +1344,8 @@
   </sheetPr>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1474,9 +1474,7 @@
       <c r="A8" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="B8" s="17" t="s">
-        <v>37</v>
-      </c>
+      <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
       <c r="E8" s="17"/>
@@ -2149,10 +2147,10 @@
   <sheetPr>
     <tabColor theme="5"/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,14 +2182,6 @@
       </c>
       <c r="G1" s="10" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>91</v>
       </c>
     </row>
   </sheetData>
@@ -2319,7 +2309,7 @@
   </sheetPr>
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>